<commit_message>
oeloginpage implementation and updated testng.xml file
</commit_message>
<xml_diff>
--- a/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
+++ b/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\DCPLProjectOrderExecution\DCPLProjectOrderExecution\src\test\resources\TestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908E77B2-77A7-460E-BDE7-7629035FAC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="OELogin" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +24,26 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+  <si>
+    <t>hrms_id</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>Pass@123</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +51,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,14 +90,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +395,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{92841F9F-5DB1-4605-BB6E-C56355093625}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test script written for PSQ Floor Percentage Create,Search<edit and Delete
</commit_message>
<xml_diff>
--- a/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
+++ b/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\DCPLProjectOrderExecution\DCPLProjectOrderExecution\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908E77B2-77A7-460E-BDE7-7629035FAC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBE9C3A-E647-4E95-9AF3-BA30113FE55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OELogin" sheetId="1" r:id="rId1"/>
+    <sheet name="ReleaseOrder" sheetId="2" r:id="rId2"/>
+    <sheet name="PSQFloorPercentage" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
   <si>
     <t>hrms_id</t>
   </si>
@@ -37,6 +40,102 @@
   </si>
   <si>
     <t>110</t>
+  </si>
+  <si>
+    <t>StoreCode</t>
+  </si>
+  <si>
+    <t>OrderNo</t>
+  </si>
+  <si>
+    <t>OrderType</t>
+  </si>
+  <si>
+    <t>Vendor</t>
+  </si>
+  <si>
+    <t>Segment</t>
+  </si>
+  <si>
+    <t>OrderKind</t>
+  </si>
+  <si>
+    <t>TS Madision</t>
+  </si>
+  <si>
+    <t>BKK - BALKISHORE KHANNA AND COMPANY</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>New Order-NO</t>
+  </si>
+  <si>
+    <t>Customer Order</t>
+  </si>
+  <si>
+    <t>48608</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CKCCO-C. Krishniah Chetty &amp; Co. Private Limited </t>
+  </si>
+  <si>
+    <t>region</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>grade</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>storename</t>
+  </si>
+  <si>
+    <t>segment</t>
+  </si>
+  <si>
+    <t>floorpercentage</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>2023</t>
+  </si>
+  <si>
+    <t>is_active</t>
+  </si>
+  <si>
+    <t>Valuator</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>editfloorpercentagevalue</t>
+  </si>
+  <si>
+    <t>75</t>
   </si>
 </sst>
 </file>
@@ -110,11 +209,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -398,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -426,4 +526,192 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF3E46F-F8D0-4226-8102-106540E6973E}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="4" max="4" width="37.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{9F815AE1-F8DA-48E2-9027-FA2A641E760D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1D3B09-9E60-4903-A9D5-6C9C9EFA5378}">
+  <dimension ref="A1:M2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="41.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.21875" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+    <col min="13" max="13" width="22.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4CD2E0A2-C573-4073-BCE9-28F7FB3F565E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
for new chrome driver
</commit_message>
<xml_diff>
--- a/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
+++ b/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\DCPLProjectOrderExecution\DCPLProjectOrderExecution\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBE9C3A-E647-4E95-9AF3-BA30113FE55B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C10603C-BB5A-4DCB-A15D-BDBDACD7DE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OELogin" sheetId="1" r:id="rId1"/>
     <sheet name="ReleaseOrder" sheetId="2" r:id="rId2"/>
     <sheet name="PSQFloorPercentage" sheetId="3" r:id="rId3"/>
+    <sheet name="PSQTarget" sheetId="4" r:id="rId4"/>
+    <sheet name="PSQAttendance" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>hrms_id</t>
   </si>
@@ -126,22 +127,73 @@
     <t>is_active</t>
   </si>
   <si>
-    <t>Valuator</t>
-  </si>
-  <si>
-    <t>Jul</t>
-  </si>
-  <si>
     <t>editfloorpercentagevalue</t>
   </si>
   <si>
     <t>75</t>
+  </si>
+  <si>
+    <t>targetsegment</t>
+  </si>
+  <si>
+    <t>includesegment</t>
+  </si>
+  <si>
+    <t>Platinum</t>
+  </si>
+  <si>
+    <t>Gold-Bangle Odd-Zone</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>targetvalue</t>
+  </si>
+  <si>
+    <t>150000.00</t>
+  </si>
+  <si>
+    <t>Supervisor</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>ADMIN</t>
+  </si>
+  <si>
+    <t>years</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>noofdayspresent</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>dcname</t>
+  </si>
+  <si>
+    <t>190</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00;[Red]0.00"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -209,12 +261,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -612,8 +667,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B1D3B09-9E60-4903-A9D5-6C9C9EFA5378}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,7 +718,7 @@
         <v>31</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -680,7 +735,7 @@
         <v>22</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>23</v>
@@ -698,13 +753,13 @@
         <v>30</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -714,4 +769,200 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE0BE0D-D673-4AFC-8982-04CC74008F16}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{FEDB3277-52EA-4D21-91FA-5EF09CC86450}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD988FC-69C9-4C18-A5A0-8C569E6B2DB5}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="H7" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F340035B-D776-495F-A153-F9A1893E9913}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Developed test script for receive parcel create.
</commit_message>
<xml_diff>
--- a/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
+++ b/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\DCPLProjectOrderExecution\DCPLProjectOrderExecution\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C10603C-BB5A-4DCB-A15D-BDBDACD7DE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FBC415-7E5A-4B11-937A-A905CF522B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OELogin" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="PSQFloorPercentage" sheetId="3" r:id="rId3"/>
     <sheet name="PSQTarget" sheetId="4" r:id="rId4"/>
     <sheet name="PSQAttendance" sheetId="5" r:id="rId5"/>
+    <sheet name="Receive Parcel" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
   <si>
     <t>hrms_id</t>
   </si>
@@ -185,6 +186,69 @@
   </si>
   <si>
     <t>190</t>
+  </si>
+  <si>
+    <t>vendor</t>
+  </si>
+  <si>
+    <t>deliverymode</t>
+  </si>
+  <si>
+    <t>materialtype</t>
+  </si>
+  <si>
+    <t>insuredamount</t>
+  </si>
+  <si>
+    <t>noofboxes</t>
+  </si>
+  <si>
+    <t>courieragencyname</t>
+  </si>
+  <si>
+    <t>courierreceiptnumber</t>
+  </si>
+  <si>
+    <t>couriercharges</t>
+  </si>
+  <si>
+    <t>borneby</t>
+  </si>
+  <si>
+    <t>grosswt</t>
+  </si>
+  <si>
+    <t>receivedby</t>
+  </si>
+  <si>
+    <t>sentby</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>25000</t>
+  </si>
+  <si>
+    <t>12345</t>
+  </si>
+  <si>
+    <t>1500</t>
+  </si>
+  <si>
+    <t>BKK</t>
   </si>
 </sst>
 </file>
@@ -261,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -269,7 +333,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -554,7 +617,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,9 +650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAF3E46F-F8D0-4226-8102-106540E6973E}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -871,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AD988FC-69C9-4C18-A5A0-8C569E6B2DB5}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -939,13 +1000,13 @@
       <c r="F2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="4" t="s">
         <v>44</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="4" t="s">
         <v>47</v>
       </c>
       <c r="J2" s="2" t="s">
@@ -965,4 +1026,108 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A830C6A-2351-42AD-9726-C7D67A089D6F}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{0631F7EA-E78A-4227-84CA-DFD8CD2BD140}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Written script for grv function
</commit_message>
<xml_diff>
--- a/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
+++ b/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\DCPLProjectOrderExecution\DCPLProjectOrderExecution\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FBC415-7E5A-4B11-937A-A905CF522B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19989D3-7526-41C4-BA74-D144F48421ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OELogin" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="PSQTarget" sheetId="4" r:id="rId4"/>
     <sheet name="PSQAttendance" sheetId="5" r:id="rId5"/>
     <sheet name="Receive Parcel" sheetId="7" r:id="rId6"/>
+    <sheet name="GRV" sheetId="8" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="125">
   <si>
     <t>hrms_id</t>
   </si>
@@ -249,6 +251,162 @@
   </si>
   <si>
     <t>BKK</t>
+  </si>
+  <si>
+    <t>grvno</t>
+  </si>
+  <si>
+    <t>grvdate</t>
+  </si>
+  <si>
+    <t>grvtype</t>
+  </si>
+  <si>
+    <t>cgstamount</t>
+  </si>
+  <si>
+    <t>sgstamount</t>
+  </si>
+  <si>
+    <t>igstamount</t>
+  </si>
+  <si>
+    <t>cessamount</t>
+  </si>
+  <si>
+    <t>regunreg</t>
+  </si>
+  <si>
+    <t>gstinno</t>
+  </si>
+  <si>
+    <t>sourcestate</t>
+  </si>
+  <si>
+    <t>invoiceamount</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>07BKKCH1747D1ZY</t>
+  </si>
+  <si>
+    <t>UnRegistered</t>
+  </si>
+  <si>
+    <t>igstPerc</t>
+  </si>
+  <si>
+    <t>segments</t>
+  </si>
+  <si>
+    <t>hsnsaccode</t>
+  </si>
+  <si>
+    <t>cgstPerc</t>
+  </si>
+  <si>
+    <t>sgstPerc</t>
+  </si>
+  <si>
+    <t>cessPerc</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>partybillno</t>
+  </si>
+  <si>
+    <t>987456</t>
+  </si>
+  <si>
+    <t>partybillMonthYear</t>
+  </si>
+  <si>
+    <t>partybillDay</t>
+  </si>
+  <si>
+    <t>January 2024</t>
+  </si>
+  <si>
+    <t>Karnataka</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>pcs</t>
+  </si>
+  <si>
+    <t>netwt</t>
+  </si>
+  <si>
+    <t>wast.wt</t>
+  </si>
+  <si>
+    <t>metalrate</t>
+  </si>
+  <si>
+    <t>diamondwt</t>
+  </si>
+  <si>
+    <t>labourcharge</t>
+  </si>
+  <si>
+    <t>valueinrs</t>
+  </si>
+  <si>
+    <t>remarks</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>4250</t>
+  </si>
+  <si>
+    <t>2500</t>
+  </si>
+  <si>
+    <t>35000</t>
+  </si>
+  <si>
+    <t>skinpurityG</t>
+  </si>
+  <si>
+    <t>parcelid</t>
+  </si>
+  <si>
+    <t>71131910</t>
+  </si>
+  <si>
+    <t>silver</t>
+  </si>
+  <si>
+    <t>platinum</t>
+  </si>
+  <si>
+    <t>diamond</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>2181</t>
   </si>
 </sst>
 </file>
@@ -325,7 +483,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -333,6 +491,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1032,8 +1193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A830C6A-2351-42AD-9726-C7D67A089D6F}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1130,4 +1291,283 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DEDDC4C-1822-423E-A6B2-E3DFEA3895E6}">
+  <dimension ref="A1:AI2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6640625" customWidth="1"/>
+    <col min="15" max="15" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.33203125" customWidth="1"/>
+    <col min="24" max="24" width="17.109375" customWidth="1"/>
+    <col min="25" max="25" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="H2" s="4">
+        <v>100</v>
+      </c>
+      <c r="I2" s="4">
+        <v>100</v>
+      </c>
+      <c r="J2" s="4">
+        <v>200</v>
+      </c>
+      <c r="K2" s="4">
+        <v>50</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="O2" s="7">
+        <v>5000</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AG2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AH2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AI2" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D2AEE2C7-B5C3-441D-89DA-9C53CF82A3A0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA81FF2F-75FC-4FD6-941C-6B1DC60F5CCF}">
+  <dimension ref="F18:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="18" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>120</v>
+      </c>
+      <c r="H18">
+        <v>71131130</v>
+      </c>
+    </row>
+    <row r="19" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>121</v>
+      </c>
+      <c r="H19">
+        <v>71131950</v>
+      </c>
+    </row>
+    <row r="20" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>122</v>
+      </c>
+      <c r="H20">
+        <v>71131930</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
new test cases script has been written for platinum,silver,diamond,ls and accessory
</commit_message>
<xml_diff>
--- a/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
+++ b/DCPLProjectOrderExecution/src/test/resources/TestData/OETestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\git\DCPLProjectOrderExecution\DCPLProjectOrderExecution\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19989D3-7526-41C4-BA74-D144F48421ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6036AB9F-87EC-456C-A7F9-786B393245D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OELogin" sheetId="1" r:id="rId1"/>
@@ -1193,11 +1193,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A830C6A-2351-42AD-9726-C7D67A089D6F}">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
@@ -1297,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DEDDC4C-1822-423E-A6B2-E3DFEA3895E6}">
   <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>